<commit_message>
[WRITE] Correciones a modo potencia
</commit_message>
<xml_diff>
--- a/data/proyectos_ficticios_dashboard.xlsx
+++ b/data/proyectos_ficticios_dashboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -22,6 +22,9 @@
     <t>nombre_proyecto</t>
   </si>
   <si>
+    <t>descripcion</t>
+  </si>
+  <si>
     <t>multiplicador de empleo</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t>Doble calzada Barranquilla – Ciénaga</t>
   </si>
   <si>
+    <t>Doble calzada Barranquilla – Ciénaga  es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>INVIAS</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
     <t>Planta regional de tratamiento de residuos</t>
   </si>
   <si>
+    <t>Planta regional de tratamiento de  residuos   es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>IDEAM</t>
   </si>
   <si>
@@ -121,6 +130,9 @@
     <t>Hospital regional del Caribe</t>
   </si>
   <si>
+    <t>Hospital regional del Caribe   es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>Ministerio de Salud</t>
   </si>
   <si>
@@ -130,6 +142,9 @@
     <t>Parque solar La Guajira</t>
   </si>
   <si>
+    <t>Parque solar La Guajira   es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>Ministerio de Minas y Energía</t>
   </si>
   <si>
@@ -139,6 +154,9 @@
     <t>Universidad tecnológica del Atlántico</t>
   </si>
   <si>
+    <t>Universidad tecnológica del Atlántico   es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>Ministerio de Educación</t>
   </si>
   <si>
@@ -148,6 +166,9 @@
     <t>Acueducto rural Magdalena</t>
   </si>
   <si>
+    <t>Acueducto rural Magdalena   es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
+  </si>
+  <si>
     <t>Ministerio de Vivienda</t>
   </si>
   <si>
@@ -155,6 +176,9 @@
   </si>
   <si>
     <t>Centro cultural del Pacífico</t>
+  </si>
+  <si>
+    <t>Centro cultural del Pacífico  es un proyecto que busca tener grandes avances en la gestión y consolidación de beneficios para la ciudadania en general por medio de la exploracion.</t>
   </si>
   <si>
     <t>Ministerio de Cultura</t>
@@ -216,16 +240,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -538,47 +559,48 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="38.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -587,13 +609,13 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -646,6 +668,9 @@
       </c>
       <c r="Y1" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -653,76 +678,79 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3">
         <v>131376</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="3">
         <v>1500</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="3">
         <v>2247000</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3">
         <v>2572586</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -730,76 +758,79 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>400</v>
+      </c>
+      <c r="F3" s="3">
+        <v>850000</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2548578</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4">
-        <v>4500</v>
-      </c>
-      <c r="D3" s="4">
-        <v>400</v>
-      </c>
-      <c r="E3" s="4">
-        <v>850000</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="4">
-        <v>2548578</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="O3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -807,76 +838,79 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3">
         <v>12000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="3">
         <v>800</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="3">
         <v>450000</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="3">
         <v>2549001</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -884,76 +918,79 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="4">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3">
         <v>7500</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="3">
         <v>1200</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="3">
         <v>300000</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3">
         <v>2549002</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -961,76 +998,79 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="4">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
         <v>9500</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="3">
         <v>950</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="3">
         <v>120000</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="3">
         <v>2549003</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -1038,76 +1078,79 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3">
         <v>3500</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="3">
         <v>600</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="3">
         <v>80000</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="3">
         <v>2549004</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -1115,76 +1158,79 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="4">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="3">
         <v>5000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="3">
         <v>700</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="3">
         <v>150000</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3">
         <v>2549005</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>